<commit_message>
Made second window look better
</commit_message>
<xml_diff>
--- a/FINAL_PLAYLIST.xlsx
+++ b/FINAL_PLAYLIST.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,15 +551,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>spotify:track:6dxIYR9BLsRtbV9WmVlb29</t>
+          <t>spotify:track:4nlvKIIetOWGIMyhjQXgOZ</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2021-01-15T13:17:32Z</t>
+          <t>2020-03-30T15:50:21Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -569,11 +569,11 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.19042; x64)</t>
+          <t>Windows 10 (10.0.18362; x64; AppX)</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>647095</v>
+        <v>139662</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -582,7 +582,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -592,17 +592,17 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Afraid of Us</t>
+          <t>The Difference</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Jonwayne</t>
+          <t>Flume</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Rap Album Two</t>
+          <t>The Difference</t>
         </is>
       </c>
       <c r="N2" t="inlineStr"/>
@@ -610,7 +610,7 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>fwdbtn</t>
+          <t>clickrow</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>1610715714042</v>
+        <v>1585579289734</v>
       </c>
       <c r="W2" t="b">
         <v>0</v>
@@ -634,19 +634,19 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>spotify:track:5IafdoRLyaGPeeA6f8ysIe</t>
+          <t>spotify:track:7zIUcWKZuaQFWitgICgqxy</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2021-01-28T17:57:07Z</t>
+          <t>2020-03-30T21:22:14Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -656,11 +656,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.19042; x64)</t>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>118933</v>
+        <v>183854</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -669,7 +669,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>31.187.0.247</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -679,17 +679,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>I'm So Tired</t>
+          <t>Robbin Szn</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Fugazi</t>
+          <t>Tebi Rex</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Instrument Soundtrack</t>
+          <t>The Young Will Eat The Old</t>
         </is>
       </c>
       <c r="N3" t="inlineStr"/>
@@ -713,7 +713,7 @@
         <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>1611856506865</v>
+        <v>1585603141286</v>
       </c>
       <c r="W3" t="b">
         <v>0</v>
@@ -721,19 +721,19 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>spotify:track:587yWjYOx7VVGyeI9m574a</t>
+          <t>spotify:track:6gw6tt40BdB8E3mmLsrkHJ</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2021-01-03T16:57:01Z</t>
+          <t>2020-03-30T19:29:14Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -743,11 +743,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Windows 10 (10.0.18362; x64; AppX)</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>214595</v>
+        <v>29600</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -756,7 +756,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -766,17 +766,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Digital Baptism</t>
+          <t>Cannibal Tree</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Falconite</t>
+          <t>Yenkee</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Digital Baptism</t>
+          <t>Cannibal Tree</t>
         </is>
       </c>
       <c r="N4" t="inlineStr"/>
@@ -784,23 +784,23 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>clickrow</t>
+          <t>fwdbtn</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>endplay</t>
         </is>
       </c>
       <c r="S4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="b">
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>1609692808719</v>
+        <v>1585596525402</v>
       </c>
       <c r="W4" t="b">
         <v>0</v>
@@ -808,19 +808,19 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>spotify:track:35XB41L0gtDG2EXqMqq1wu</t>
+          <t>spotify:track:7gYyQi4sujOwX9OgDMB4Hn</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2021-01-09T00:11:45Z</t>
+          <t>2020-03-30T21:15:19Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -830,11 +830,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>263764</v>
+        <v>207272</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -843,7 +843,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>31.187.0.247</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -853,17 +853,17 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Some Minds</t>
+          <t>Lotus Eaters</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Flume</t>
+          <t>Tebi Rex</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Some Minds</t>
+          <t>The Young Will Eat The Old</t>
         </is>
       </c>
       <c r="N5" t="inlineStr"/>
@@ -871,7 +871,7 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>fwdbtn</t>
+          <t>clickrow</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -880,14 +880,14 @@
         </is>
       </c>
       <c r="S5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="b">
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>1610150842515</v>
+        <v>1585602709707</v>
       </c>
       <c r="W5" t="b">
         <v>0</v>
@@ -895,19 +895,19 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>86</v>
+        <v>121</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>spotify:track:3E9Wv5hNRwedUjPkkplcx4</t>
+          <t>spotify:track:7n6vwGiH4b0isEe7ijSDgi</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2021-01-03T17:20:45Z</t>
+          <t>2020-03-27T05:51:52Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -917,11 +917,11 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>3495</v>
+        <v>329863</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -930,7 +930,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -940,17 +940,17 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Not Dead Yet</t>
+          <t>Live It</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Jakey</t>
+          <t>Teho</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Not Dead Yet</t>
+          <t>Live It</t>
         </is>
       </c>
       <c r="N6" t="inlineStr"/>
@@ -963,7 +963,7 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>fwdbtn</t>
+          <t>logout</t>
         </is>
       </c>
       <c r="S6" t="b">
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>1609694441008</v>
+        <v>1585255110608</v>
       </c>
       <c r="W6" t="b">
         <v>0</v>
@@ -982,19 +982,19 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>101</v>
+        <v>149</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>spotify:track:6EztTMv6l0WEj7H8tIjn9i</t>
+          <t>spotify:track:02sVtQ6XBFhPauNe1aLNCZ</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2021-01-15T20:11:10Z</t>
+          <t>2020-03-20T15:09:42Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1004,11 +1004,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.19042; x64)</t>
+          <t>Windows 10 (10.0.18362; x64; AppX)</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>287356</v>
+        <v>270650</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1027,17 +1027,17 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Melody Day - Four Tet Remix</t>
+          <t>Behind Me</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Caribou</t>
+          <t>Teho</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Melody Day</t>
+          <t>Manualism 9.0</t>
         </is>
       </c>
       <c r="N7" t="inlineStr"/>
@@ -1045,12 +1045,12 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>clickrow</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>endplay</t>
         </is>
       </c>
       <c r="S7" t="b">
@@ -1061,7 +1061,7 @@
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>1610740964695</v>
+        <v>1584716637729</v>
       </c>
       <c r="W7" t="b">
         <v>0</v>
@@ -1069,19 +1069,19 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>116</v>
+        <v>175</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>spotify:track:50TPDl3f8XCAyFMj9k0fit</t>
+          <t>spotify:track:3VIJBrMpvimHEw5wtPh2wB</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2021-01-02T19:22:09Z</t>
+          <t>2020-04-12T18:40:19Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1095,7 +1095,7 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>172803</v>
+        <v>233639</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1114,17 +1114,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Lamborghini Meltdown</t>
+          <t>Money</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>DEMON QUEEN</t>
+          <t>The Drums</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Exorcise Tape</t>
+          <t>Portamento</t>
         </is>
       </c>
       <c r="N8" t="inlineStr"/>
@@ -1132,7 +1132,7 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>playbtn</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>1609615157055</v>
+        <v>1586716584072</v>
       </c>
       <c r="W8" t="b">
         <v>0</v>
@@ -1156,19 +1156,19 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>130</v>
+        <v>201</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>spotify:track:53XM8O6sQ4YzCq2jYgXuC6</t>
+          <t>spotify:track:2cYALQZNXmuFGp2ecgpKMa</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2021-01-28T15:52:24Z</t>
+          <t>2020-03-22T20:57:33Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1178,11 +1178,11 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Android OS 10 API 29 (OnePlus, HD1903)</t>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>28691</v>
+        <v>204066</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>31.187.2.139</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1201,17 +1201,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Cyclone (The Village Sessions)</t>
+          <t>cellophane</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Sticky Fingers</t>
+          <t>FKA twigs</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Cyclone (The Village Sessions)</t>
+          <t>MAGDALENE</t>
         </is>
       </c>
       <c r="N9" t="inlineStr"/>
@@ -1224,7 +1224,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>logout</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="S9" t="b">
@@ -1235,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>1611849017632</v>
+        <v>1584910257868</v>
       </c>
       <c r="W9" t="b">
         <v>0</v>
@@ -1243,19 +1243,19 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>143</v>
+        <v>226</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>spotify:track:3Bz3lj6E9VFBk1Wj1hC8vw</t>
+          <t>spotify:track:0BBB7WOLQPEdUZRR23WwQ8</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2021-01-02T19:26:07Z</t>
+          <t>2020-05-09T21:57:17Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1269,7 +1269,7 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>237726</v>
+        <v>179775</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -1278,7 +1278,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1288,17 +1288,17 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Sleeping Lessons</t>
+          <t>Retrograde</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>The Shins</t>
+          <t>Lexkriix</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Wincing The Night Away</t>
+          <t>Beats Sound</t>
         </is>
       </c>
       <c r="N10" t="inlineStr"/>
@@ -1306,7 +1306,7 @@
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>clickrow</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1315,14 +1315,14 @@
         </is>
       </c>
       <c r="S10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="b">
         <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>1609615329543</v>
+        <v>1589061257430</v>
       </c>
       <c r="W10" t="b">
         <v>0</v>
@@ -1330,19 +1330,19 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>156</v>
+        <v>249</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>spotify:track:0bu2J9iVXDYUyYoLWbQfjl</t>
+          <t>spotify:track:5Y8UUyWfuQ0EAmYLvwwcJL</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2021-01-14T19:15:57Z</t>
+          <t>2020-03-22T21:01:19Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1352,11 +1352,11 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Android OS 10 API 29 (OnePlus, HD1903)</t>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>12880</v>
+        <v>224946</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1375,17 +1375,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Metroma</t>
+          <t>home with you</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>The Sei</t>
+          <t>FKA twigs</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Metroma</t>
+          <t>MAGDALENE</t>
         </is>
       </c>
       <c r="N11" t="inlineStr"/>
@@ -1393,12 +1393,12 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>clickrow</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>logout</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="S11" t="b">
@@ -1409,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>1610628899747</v>
+        <v>1584910652957</v>
       </c>
       <c r="W11" t="b">
         <v>0</v>
@@ -1417,19 +1417,19 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>166</v>
+        <v>271</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>spotify:track:71rhKCdkNgUgHCMMiMeuKJ</t>
+          <t>spotify:track:1aayZc3JciIs2GhZcSlCrw</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2021-01-03T16:58:10Z</t>
+          <t>2020-04-13T19:57:49Z</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1443,7 +1443,7 @@
         </is>
       </c>
       <c r="G12" t="n">
-        <v>67494</v>
+        <v>272039</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1452,7 +1452,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1462,17 +1462,17 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>MARBLE TEA</t>
+          <t>We're Finally Landing</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Shawn Wasabi</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>MANGOTALE</t>
+          <t>Before the Night</t>
         </is>
       </c>
       <c r="N12" t="inlineStr"/>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>endplay</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="S12" t="b">
@@ -1496,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="V12" t="n">
-        <v>1609693022668</v>
+        <v>1586807596291</v>
       </c>
       <c r="W12" t="b">
         <v>0</v>
@@ -1504,19 +1504,19 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>176</v>
+        <v>292</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>spotify:track:1iDbUIQcRyUpl1K1WPZOVW</t>
+          <t>spotify:track:6m5SxiI5o8oRgtARg0Oneq</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2021-01-07T13:07:02Z</t>
+          <t>2020-04-17T22:21:23Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1530,7 +1530,7 @@
         </is>
       </c>
       <c r="G13" t="n">
-        <v>145108</v>
+        <v>213968</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1549,17 +1549,17 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Go Like - D&amp;B Remix</t>
+          <t>For Ants</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Fox Stevenson</t>
+          <t>Yuri Wong</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Go Like (D&amp;B Mix)</t>
+          <t>For Ants</t>
         </is>
       </c>
       <c r="N13" t="inlineStr"/>
@@ -1567,12 +1567,12 @@
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>fwdbtn</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>remote</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="S13" t="b">
@@ -1583,7 +1583,7 @@
         <v>0</v>
       </c>
       <c r="V13" t="n">
-        <v>1609957602290</v>
+        <v>1587161869307</v>
       </c>
       <c r="W13" t="b">
         <v>0</v>
@@ -1591,19 +1591,19 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>186</v>
+        <v>312</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>spotify:track:786ymAh5BmHoIpvjyrvjXk</t>
+          <t>spotify:track:1JO6GZPZ1sVTuIsxXSSo1w</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2021-01-03T17:11:55Z</t>
+          <t>2020-04-27T20:33:32Z</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="G14" t="n">
-        <v>328506</v>
+        <v>421883</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1636,17 +1636,17 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Goodbye To A World</t>
+          <t>The Flute Tune (Soulpride Remix)</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Porter Robinson</t>
+          <t>Jaycut</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Worlds</t>
+          <t>Jaycut &amp; Kolt Siewerts - The Flute Tune (Soulpride Remix)</t>
         </is>
       </c>
       <c r="N14" t="inlineStr"/>
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>1609693091620</v>
+        <v>1588010604608</v>
       </c>
       <c r="W14" t="b">
         <v>0</v>
@@ -1678,19 +1678,19 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>195</v>
+        <v>332</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>spotify:track:1SN1gifVAKecU85lZggS8k</t>
+          <t>spotify:track:1uKmDqnJWzbmcugkIpTThd</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2021-01-02T19:50:01Z</t>
+          <t>2020-04-20T13:31:22Z</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1700,11 +1700,11 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>282853</v>
+        <v>174803</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1723,17 +1723,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>No Reptiles</t>
+          <t>Alone - Unplugged</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Everything Everything</t>
+          <t>sayk_</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Get To Heaven (Deluxe)</t>
+          <t>404</t>
         </is>
       </c>
       <c r="N15" t="inlineStr"/>
@@ -1741,7 +1741,7 @@
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>clickrow</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1757,7 +1757,7 @@
         <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>1609616718522</v>
+        <v>1587389307607</v>
       </c>
       <c r="W15" t="b">
         <v>0</v>
@@ -1765,19 +1765,19 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>203</v>
+        <v>352</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>spotify:track:5PycJHxshGJkLaNm9TV9xk</t>
+          <t>spotify:track:1QZOVF6AqgEiqoWdhcJvYo</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2021-01-15T16:15:14Z</t>
+          <t>2020-03-15T00:46:50Z</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1787,11 +1787,11 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.19042; x64)</t>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>94704</v>
+        <v>3640</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1810,17 +1810,17 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Green Light</t>
+          <t>I’m Not Human at All</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Jonwayne</t>
+          <t>Sleep Party People</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Jonwayne is Retired</t>
+          <t>Sleep Party People</t>
         </is>
       </c>
       <c r="N16" t="inlineStr"/>
@@ -1828,12 +1828,12 @@
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>clickrow</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>remote</t>
+          <t>fwdbtn</t>
         </is>
       </c>
       <c r="S16" t="b">
@@ -1844,7 +1844,7 @@
         <v>0</v>
       </c>
       <c r="V16" t="n">
-        <v>1610716651727</v>
+        <v>1584233204580</v>
       </c>
       <c r="W16" t="b">
         <v>0</v>
@@ -1852,19 +1852,19 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>210</v>
+        <v>371</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>spotify:track:0BxE4FqsDD1Ot4YuBXwAPp</t>
+          <t>spotify:track:32k4CnRS4iY74LDeyeDBnl</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2021-01-02T19:30:21Z</t>
+          <t>2020-03-02T15:21:40Z</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1874,11 +1874,11 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>253586</v>
+        <v>152154</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>143.239.9.6</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1897,17 +1897,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>505</t>
+          <t>I Can Feel It in My Bones</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Arctic Monkeys</t>
+          <t>Æ MAK</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>Favourite Worst Nightmare</t>
+          <t>I Can Feel It in My Bones</t>
         </is>
       </c>
       <c r="N17" t="inlineStr"/>
@@ -1931,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="V17" t="n">
-        <v>1609615567765</v>
+        <v>1583162346183</v>
       </c>
       <c r="W17" t="b">
         <v>0</v>
@@ -1939,19 +1939,19 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>217</v>
+        <v>388</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>spotify:track:3Bj2mrlp3tALHO5U3mK8zM</t>
+          <t>spotify:track:3kNaNDh2G5Q9jAXpqoA51b</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2021-01-02T19:34:10Z</t>
+          <t>2020-03-30T21:19:03Z</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1961,11 +1961,11 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>228019</v>
+        <v>223448</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>31.187.0.247</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Blade Runner 2049</t>
+          <t>I Never Got Off The Bus</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Synthwave Goose</t>
+          <t>Tebi Rex</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Blade Runner 2049</t>
+          <t>The Young Will Eat The Old</t>
         </is>
       </c>
       <c r="N18" t="inlineStr"/>
@@ -2018,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="V18" t="n">
-        <v>1609615821862</v>
+        <v>1585602917349</v>
       </c>
       <c r="W18" t="b">
         <v>0</v>
@@ -2026,19 +2026,19 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>224</v>
+        <v>404</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>spotify:track:6muCGaU3LBXVbArWupCmrB</t>
+          <t>spotify:track:45m6ioYnsSA5TeY6EE82Ha</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2021-01-02T19:45:18Z</t>
+          <t>2020-03-02T15:19:07Z</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -2048,11 +2048,11 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>231893</v>
+        <v>173357</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>143.239.9.6</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -2071,17 +2071,17 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Arch Enemy</t>
+          <t>Dancing Bug</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Everything Everything</t>
+          <t>Le Boom</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>RE-ANIMATOR</t>
+          <t>Dancing Bug</t>
         </is>
       </c>
       <c r="N19" t="inlineStr"/>
@@ -2089,7 +2089,7 @@
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>clickrow</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2105,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="V19" t="n">
-        <v>1609616486133</v>
+        <v>1583162173916</v>
       </c>
       <c r="W19" t="b">
         <v>0</v>
@@ -2113,19 +2113,19 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>230</v>
+        <v>420</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>spotify:track:0nrRP2bk19rLc0orkWPQk2</t>
+          <t>spotify:track:5ypOQL3PMZJoBkS2HMPCXO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2021-01-23T16:11:29Z</t>
+          <t>2020-04-17T00:46:57Z</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -2135,11 +2135,11 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Android OS 10 API 29 (OnePlus, HD1903)</t>
+          <t>Windows 10 (10.0.18363; x64; AppX)</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>3795</v>
+        <v>244148</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -2148,7 +2148,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -2158,17 +2158,17 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Wake Me Up</t>
+          <t>Really Happy Aliens</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Avicii</t>
+          <t>Fred V</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>Proximity</t>
         </is>
       </c>
       <c r="N20" t="inlineStr"/>
@@ -2176,12 +2176,12 @@
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>fwdbtn</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>remote</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="S20" t="b">
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="V20" t="n">
-        <v>1611418284285</v>
+        <v>1587084172222</v>
       </c>
       <c r="W20" t="b">
         <v>0</v>
@@ -2200,19 +2200,19 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>236</v>
+        <v>435</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>spotify:track:1R8kvV2AgNPCA2Pp4Im1Ao</t>
+          <t>spotify:track:3tjwjBfPO1pyjhnrI0J5Nq</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2021-01-13T23:48:27Z</t>
+          <t>2020-04-13T20:05:34Z</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2222,11 +2222,11 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.19042; x64)</t>
+          <t>Windows 10 (10.0.18363; x64; AppX)</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>291317</v>
+        <v>213132</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>80.111.96.121</t>
+          <t>109.255.113.201</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2245,17 +2245,17 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Baby Hotline</t>
+          <t>Head First</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Jack Stauber's Micropop</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Baby Hotline / Tea Errors</t>
+          <t>Falling into Place</t>
         </is>
       </c>
       <c r="N21" t="inlineStr"/>
@@ -2263,7 +2263,7 @@
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>clickrow</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2279,9 +2279,879 @@
         <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>1610581416554</v>
+        <v>1586808120333</v>
       </c>
       <c r="W21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>449</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>spotify:track:3mxEfSqWVcQBHxMLHxv5r1</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>14</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2020-03-15T14:01:29Z</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>11120906237</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>590</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>109.255.113.201</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>I'm Not Human At All (Copenhagen X Sessions)</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Sleep Party People</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>I'm Not Human At All (Copenhagen X Sessions)</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>fwdbtn</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>unexpected-exit-while-paused</t>
+        </is>
+      </c>
+      <c r="S22" t="b">
+        <v>0</v>
+      </c>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="b">
+        <v>0</v>
+      </c>
+      <c r="V22" t="n">
+        <v>1584233209694</v>
+      </c>
+      <c r="W22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>463</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>spotify:track:7ympnDShDtkevRDPxMqPvR</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>14</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2020-05-10T21:03:55Z</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>11120906237</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Windows 10 (10.0.18362; x64; AppX)</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>471946</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>109.255.113.201</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Winter on the Weekend</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Julia Stone</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>The Memory Machine</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>clickrow</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>trackdone</t>
+        </is>
+      </c>
+      <c r="S23" t="b">
+        <v>0</v>
+      </c>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="b">
+        <v>0</v>
+      </c>
+      <c r="V23" t="n">
+        <v>1589143516197</v>
+      </c>
+      <c r="W23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>477</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>spotify:track:3JvJupyJyXk9aWtSXyZqcc</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>13</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2020-03-22T21:05:22Z</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>11120906237</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>243000</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>109.255.113.201</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>holy terrain</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>FKA twigs</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>MAGDALENE</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>trackdone</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>trackdone</t>
+        </is>
+      </c>
+      <c r="S24" t="b">
+        <v>0</v>
+      </c>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="b">
+        <v>0</v>
+      </c>
+      <c r="V24" t="n">
+        <v>1584910878324</v>
+      </c>
+      <c r="W24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>490</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>spotify:track:2tRMhAhbVKb3ay9lABihPt</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>13</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2020-04-28T00:56:03Z</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>11120906237</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Windows 10 (10.0.18362; x64; AppX)</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>445735</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>109.255.113.201</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Epilogue</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Weltmusik</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Epilogue</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>trackdone</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>trackdone</t>
+        </is>
+      </c>
+      <c r="S25" t="b">
+        <v>0</v>
+      </c>
+      <c r="T25" t="inlineStr"/>
+      <c r="U25" t="b">
+        <v>0</v>
+      </c>
+      <c r="V25" t="n">
+        <v>1588034757064</v>
+      </c>
+      <c r="W25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>503</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>spotify:track:4KfgBq7SrmjavjQS4ZQGHC</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>13</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2020-03-22T21:09:49Z</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>11120906237</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>255720</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>109.255.113.201</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>sad day</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>FKA twigs</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>MAGDALENE</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>trackdone</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>trackdone</t>
+        </is>
+      </c>
+      <c r="S26" t="b">
+        <v>0</v>
+      </c>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" t="b">
+        <v>0</v>
+      </c>
+      <c r="V26" t="n">
+        <v>1584911121767</v>
+      </c>
+      <c r="W26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>516</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>spotify:track:1lCb4eleZgc8DKrv7MY21F</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>13</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2020-03-02T15:29:26Z</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>11120906237</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>244965</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>143.239.9.6</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>I Walk</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Æ MAK</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>I Walk</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>trackdone</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>trackdone</t>
+        </is>
+      </c>
+      <c r="S27" t="b">
+        <v>0</v>
+      </c>
+      <c r="T27" t="inlineStr"/>
+      <c r="U27" t="b">
+        <v>0</v>
+      </c>
+      <c r="V27" t="n">
+        <v>1583162719310</v>
+      </c>
+      <c r="W27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>529</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>spotify:track:24upABZ8A0sAepfu91sEYr</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>12</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2020-03-03T15:14:02Z</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>11120906237</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>337314</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>143.239.9.6</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Moon (And It Went Like)</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Kid Francescoli</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Play Me Again</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>clickrow</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>logout</t>
+        </is>
+      </c>
+      <c r="S28" t="b">
+        <v>0</v>
+      </c>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="b">
+        <v>0</v>
+      </c>
+      <c r="V28" t="n">
+        <v>1583227973011</v>
+      </c>
+      <c r="W28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>541</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>spotify:track:7CVV0sfN38TC3c9DaxR2Tp</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>12</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2020-03-30T21:45:54Z</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>11120906237</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Windows 10 (10.0.18362; x64; AppX)</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>121470</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>109.255.113.201</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Antenna</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Citrus Fresh</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Early Days/Late Nights</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>fwdbtn</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>endplay</t>
+        </is>
+      </c>
+      <c r="S29" t="b">
+        <v>0</v>
+      </c>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" t="b">
+        <v>0</v>
+      </c>
+      <c r="V29" t="n">
+        <v>1585601990213</v>
+      </c>
+      <c r="W29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>553</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>spotify:track:6udA6tzAZ2bolSfaSibQEV</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>11</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2020-03-09T21:42:30Z</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>11120906237</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>353407</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>109.255.113.201</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Pay Phone</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Fantom '87</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>Discovery</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>trackdone</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>trackdone</t>
+        </is>
+      </c>
+      <c r="S30" t="b">
+        <v>0</v>
+      </c>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="b">
+        <v>0</v>
+      </c>
+      <c r="V30" t="n">
+        <v>1583789795250</v>
+      </c>
+      <c r="W30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>564</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>spotify:track:7rWxjGLtUSmdr0d7X8L5Lq</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>11</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2020-03-30T21:23:41Z</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>11120906237</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>91403</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>31.187.0.247</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Men Are Trash</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Tebi Rex</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>Welcome to the Darkest Year of Our Adventures</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>trackdone</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>fwdbtn</t>
+        </is>
+      </c>
+      <c r="S31" t="b">
+        <v>0</v>
+      </c>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" t="b">
+        <v>0</v>
+      </c>
+      <c r="V31" t="n">
+        <v>1585603325763</v>
+      </c>
+      <c r="W31" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed uk us dates
</commit_message>
<xml_diff>
--- a/FINAL_PLAYLIST.xlsx
+++ b/FINAL_PLAYLIST.xlsx
@@ -551,15 +551,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>spotify:track:4nlvKIIetOWGIMyhjQXgOZ</t>
+          <t>spotify:track:0JP9xo3adEtGSdUEISiszL</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2020-03-30T15:50:21Z</t>
+          <t>2018-04-04T00:20:59Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -569,11 +569,11 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18362; x64; AppX)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>139662</v>
+        <v>135090</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -582,7 +582,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -592,17 +592,17 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>The Difference</t>
+          <t>Moonlight</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Flume</t>
+          <t>XXXTENTACION</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>The Difference</t>
+          <t>?</t>
         </is>
       </c>
       <c r="N2" t="inlineStr"/>
@@ -610,7 +610,7 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>clickrow</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>1585579289734</v>
+        <v>1522801122073</v>
       </c>
       <c r="W2" t="b">
         <v>0</v>
@@ -634,19 +634,19 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>spotify:track:7zIUcWKZuaQFWitgICgqxy</t>
+          <t>spotify:track:4Ed5gtBYbVldOnCiDcQrvf</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2020-03-30T21:22:14Z</t>
+          <t>2018-03-31T23:26:16Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -656,11 +656,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>183854</v>
+        <v>174785</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -669,7 +669,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>31.187.0.247</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -679,17 +679,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Robbin Szn</t>
+          <t>demons in my orbit</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Tebi Rex</t>
+          <t>guardin</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>The Young Will Eat The Old</t>
+          <t>demons in my orbit</t>
         </is>
       </c>
       <c r="N3" t="inlineStr"/>
@@ -697,7 +697,7 @@
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>clickrow</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -713,7 +713,7 @@
         <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>1585603141286</v>
+        <v>1522538603555</v>
       </c>
       <c r="W3" t="b">
         <v>0</v>
@@ -721,19 +721,19 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>spotify:track:6gw6tt40BdB8E3mmLsrkHJ</t>
+          <t>spotify:track:474I5bhxMtzky69EftO7lC</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2020-03-30T19:29:14Z</t>
+          <t>2018-03-29T20:05:38Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -743,11 +743,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18362; x64; AppX)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>29600</v>
+        <v>174576</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -756,7 +756,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>31.187.2.30</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -766,17 +766,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Cannibal Tree</t>
+          <t>into the trees</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Yenkee</t>
+          <t>guardin</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Cannibal Tree</t>
+          <t>into the trees</t>
         </is>
       </c>
       <c r="N4" t="inlineStr"/>
@@ -784,23 +784,23 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>fwdbtn</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>endplay</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="S4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="b">
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>1585596525402</v>
+        <v>1522353763682</v>
       </c>
       <c r="W4" t="b">
         <v>0</v>
@@ -808,19 +808,19 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>93</v>
+        <v>190</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>spotify:track:7gYyQi4sujOwX9OgDMB4Hn</t>
+          <t>spotify:track:3ieFiBzm66bZK8EwB1YNQY</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2020-03-30T21:15:19Z</t>
+          <t>2018-04-09T15:38:45Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -830,11 +830,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Windows 7 (6.1.7600; x64)</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>207272</v>
+        <v>171373</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -843,7 +843,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>31.187.0.247</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -853,17 +853,17 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Lotus Eaters</t>
+          <t>In Cold Blood (feat. Pusha T) - Baauer Remix</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Tebi Rex</t>
+          <t>alt-J</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>The Young Will Eat The Old</t>
+          <t>In Cold Blood</t>
         </is>
       </c>
       <c r="N5" t="inlineStr"/>
@@ -871,7 +871,7 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>clickrow</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -880,14 +880,14 @@
         </is>
       </c>
       <c r="S5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="b">
         <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>1585602709707</v>
+        <v>1523288065795</v>
       </c>
       <c r="W5" t="b">
         <v>0</v>
@@ -895,19 +895,19 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>121</v>
+        <v>249</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>spotify:track:7n6vwGiH4b0isEe7ijSDgi</t>
+          <t>spotify:track:4q1q6kCMwDf5YUsOkTPBLE</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2020-03-27T05:51:52Z</t>
+          <t>2018-05-01T15:38:28Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -917,11 +917,11 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>329863</v>
+        <v>346266</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -930,7 +930,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -940,17 +940,17 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Live It</t>
+          <t>Starve The Ego, Feed The Soul</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Teho</t>
+          <t>The Glitch Mob</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Live It</t>
+          <t>Drink the Sea</t>
         </is>
       </c>
       <c r="N6" t="inlineStr"/>
@@ -963,18 +963,18 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>logout</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="S6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="b">
         <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>1585255110608</v>
+        <v>1525188762331</v>
       </c>
       <c r="W6" t="b">
         <v>0</v>
@@ -982,19 +982,19 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>149</v>
+        <v>297</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>spotify:track:02sVtQ6XBFhPauNe1aLNCZ</t>
+          <t>spotify:track:2fIUrjjH7b5tQ5gnKDtb0C</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2020-03-20T15:09:42Z</t>
+          <t>2018-03-31T23:31:41Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1004,11 +1004,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18362; x64; AppX)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>270650</v>
+        <v>191429</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1027,17 +1027,17 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Behind Me</t>
+          <t>it rained &amp; it poured</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Teho</t>
+          <t>guardin</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Manualism 9.0</t>
+          <t>it rained &amp; it poured</t>
         </is>
       </c>
       <c r="N7" t="inlineStr"/>
@@ -1045,12 +1045,12 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>clickrow</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>endplay</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="S7" t="b">
@@ -1061,7 +1061,7 @@
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>1584716637729</v>
+        <v>1522538775202</v>
       </c>
       <c r="W7" t="b">
         <v>0</v>
@@ -1069,19 +1069,19 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>175</v>
+        <v>345</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>spotify:track:3VIJBrMpvimHEw5wtPh2wB</t>
+          <t>spotify:track:0or0gNaKAXYYCsOrpvRzAu</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2020-04-12T18:40:19Z</t>
+          <t>2018-04-16T21:59:49Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1091,11 +1091,11 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>233639</v>
+        <v>171727</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1114,17 +1114,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Money</t>
+          <t>Liability</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>The Drums</t>
+          <t>Lorde</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Portamento</t>
+          <t>Melodrama</t>
         </is>
       </c>
       <c r="N8" t="inlineStr"/>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>1586716584072</v>
+        <v>1523915811361</v>
       </c>
       <c r="W8" t="b">
         <v>0</v>
@@ -1156,19 +1156,19 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>201</v>
+        <v>393</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>spotify:track:2cYALQZNXmuFGp2ecgpKMa</t>
+          <t>spotify:track:4PANCoXZX3RaT2D6mqSdEU</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2020-03-22T20:57:33Z</t>
+          <t>2018-03-05T23:58:18Z</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1178,11 +1178,11 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Windows 10 (10.0.16299; x64)</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>204066</v>
+        <v>121969</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1201,17 +1201,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>cellophane</t>
+          <t>changes</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>FKA twigs</t>
+          <t>XXXTENTACION</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>MAGDALENE</t>
+          <t>changes</t>
         </is>
       </c>
       <c r="N9" t="inlineStr"/>
@@ -1219,7 +1219,7 @@
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>clickrow</t>
+          <t>appload</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1235,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>1584910257868</v>
+        <v>1520294177249</v>
       </c>
       <c r="W9" t="b">
         <v>0</v>
@@ -1243,19 +1243,19 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>226</v>
+        <v>438</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>spotify:track:0BBB7WOLQPEdUZRR23WwQ8</t>
+          <t>spotify:track:4EAV2cKiqKP5UPZmY6dejk</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2020-05-09T21:57:17Z</t>
+          <t>2018-03-20T00:34:40Z</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1265,11 +1265,11 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>179775</v>
+        <v>204746</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -1278,7 +1278,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1288,17 +1288,17 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Retrograde</t>
+          <t>Everyday</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Lexkriix</t>
+          <t>Logic</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>Beats Sound</t>
+          <t>Bobby Tarantino II</t>
         </is>
       </c>
       <c r="N10" t="inlineStr"/>
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>1589061257430</v>
+        <v>1521505877938</v>
       </c>
       <c r="W10" t="b">
         <v>0</v>
@@ -1330,19 +1330,19 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>249</v>
+        <v>482</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>spotify:track:5Y8UUyWfuQ0EAmYLvwwcJL</t>
+          <t>spotify:track:2MnI93x9Y17jJ9JAgPzTfi</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2020-03-22T21:01:19Z</t>
+          <t>2018-03-23T21:49:24Z</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1352,11 +1352,11 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>224946</v>
+        <v>233647</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1375,17 +1375,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>home with you</t>
+          <t>Where Is My Mind</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>FKA twigs</t>
+          <t>Telepathic Teddy Bear</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>MAGDALENE</t>
+          <t>Where Is My Mind</t>
         </is>
       </c>
       <c r="N11" t="inlineStr"/>
@@ -1393,7 +1393,7 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>clickrow</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1409,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>1584910652957</v>
+        <v>1521841532343</v>
       </c>
       <c r="W11" t="b">
         <v>0</v>
@@ -1417,19 +1417,19 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>271</v>
+        <v>526</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>spotify:track:1aayZc3JciIs2GhZcSlCrw</t>
+          <t>spotify:track:4nLaeAathdcgAhhB0h5aWe</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2020-04-13T19:57:49Z</t>
+          <t>2018-04-24T20:43:46Z</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1439,11 +1439,11 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>272039</v>
+        <v>217053</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1452,7 +1452,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1462,17 +1462,17 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>We're Finally Landing</t>
+          <t>Open</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Home</t>
+          <t>Rhye</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Before the Night</t>
+          <t>Woman</t>
         </is>
       </c>
       <c r="N12" t="inlineStr"/>
@@ -1480,7 +1480,7 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>clickrow</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1496,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="V12" t="n">
-        <v>1586807596291</v>
+        <v>1524602409852</v>
       </c>
       <c r="W12" t="b">
         <v>0</v>
@@ -1504,19 +1504,19 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>292</v>
+        <v>569</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>spotify:track:6m5SxiI5o8oRgtARg0Oneq</t>
+          <t>spotify:track:7nWC1XQv8bRMpVYuh5Bexj</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2020-04-17T22:21:23Z</t>
+          <t>2018-03-29T19:51:19Z</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1526,11 +1526,11 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>213968</v>
+        <v>225986</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>31.187.2.30</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1549,17 +1549,17 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>For Ants</t>
+          <t>Cowards</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Yuri Wong</t>
+          <t>Raleigh Ritchie</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>For Ants</t>
+          <t>You're a Man Now, Boy (Deluxe)</t>
         </is>
       </c>
       <c r="N13" t="inlineStr"/>
@@ -1567,7 +1567,7 @@
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>fwdbtn</t>
+          <t>clickrow</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1583,7 +1583,7 @@
         <v>0</v>
       </c>
       <c r="V13" t="n">
-        <v>1587161869307</v>
+        <v>1522352855062</v>
       </c>
       <c r="W13" t="b">
         <v>0</v>
@@ -1591,19 +1591,19 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>312</v>
+        <v>611</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>spotify:track:1JO6GZPZ1sVTuIsxXSSo1w</t>
+          <t>spotify:track:2pYvd6cHcAIMAM6xMD6nok</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2020-04-27T20:33:32Z</t>
+          <t>2018-04-24T23:03:53Z</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1613,11 +1613,11 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>421883</v>
+        <v>2862</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1636,17 +1636,17 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>The Flute Tune (Soulpride Remix)</t>
+          <t>Break Apart</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Jaycut</t>
+          <t>Bonobo</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Jaycut &amp; Kolt Siewerts - The Flute Tune (Soulpride Remix)</t>
+          <t>Migration</t>
         </is>
       </c>
       <c r="N14" t="inlineStr"/>
@@ -1654,12 +1654,12 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>clickrow</t>
+          <t>fwdbtn</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>endplay</t>
         </is>
       </c>
       <c r="S14" t="b">
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>1588010604608</v>
+        <v>1524611029154</v>
       </c>
       <c r="W14" t="b">
         <v>0</v>
@@ -1678,19 +1678,19 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>332</v>
+        <v>651</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>spotify:track:1uKmDqnJWzbmcugkIpTThd</t>
+          <t>spotify:track:2yqltlQVviRd35IqmuekLW</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2020-04-20T13:31:22Z</t>
+          <t>2018-03-20T19:50:06Z</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1700,11 +1700,11 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>174803</v>
+        <v>186945</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -1723,17 +1723,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Alone - Unplugged</t>
+          <t>The Wolf</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>sayk_</t>
+          <t>SIAMES</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>404</t>
+          <t>Bounce into the Music</t>
         </is>
       </c>
       <c r="N15" t="inlineStr"/>
@@ -1757,7 +1757,7 @@
         <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>1587389307607</v>
+        <v>1521575221573</v>
       </c>
       <c r="W15" t="b">
         <v>0</v>
@@ -1765,19 +1765,19 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>352</v>
+        <v>691</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>spotify:track:1QZOVF6AqgEiqoWdhcJvYo</t>
+          <t>spotify:track:00oy0A1Y3IS8SgP8W8xS30</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2020-03-15T00:46:50Z</t>
+          <t>2018-03-17T22:34:57Z</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1787,11 +1787,11 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Windows 10 (10.0.16299; x64)</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>3640</v>
+        <v>257266</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1800,7 +1800,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1810,17 +1810,17 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>I’m Not Human at All</t>
+          <t>Feeling Whitney</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Sleep Party People</t>
+          <t>Post Malone</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>Sleep Party People</t>
+          <t>Stoney</t>
         </is>
       </c>
       <c r="N16" t="inlineStr"/>
@@ -1828,12 +1828,12 @@
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>clickrow</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>fwdbtn</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="S16" t="b">
@@ -1844,7 +1844,7 @@
         <v>0</v>
       </c>
       <c r="V16" t="n">
-        <v>1584233204580</v>
+        <v>1521325806942</v>
       </c>
       <c r="W16" t="b">
         <v>0</v>
@@ -1852,19 +1852,19 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>371</v>
+        <v>730</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>spotify:track:32k4CnRS4iY74LDeyeDBnl</t>
+          <t>spotify:track:09EpLWJYDxbEi5VzbWA9TG</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2020-03-02T15:21:40Z</t>
+          <t>2018-03-14T18:32:42Z</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1874,11 +1874,11 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Windows 10 (10.0.16299; x64)</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>152154</v>
+        <v>168750</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>143.239.9.6</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1897,17 +1897,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>I Can Feel It in My Bones</t>
+          <t>Where Is My Mind</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Æ MAK</t>
+          <t>FMLYBND</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>I Can Feel It in My Bones</t>
+          <t>Where Is My Mind</t>
         </is>
       </c>
       <c r="N17" t="inlineStr"/>
@@ -1931,7 +1931,7 @@
         <v>0</v>
       </c>
       <c r="V17" t="n">
-        <v>1583162346183</v>
+        <v>1521052196629</v>
       </c>
       <c r="W17" t="b">
         <v>0</v>
@@ -1939,19 +1939,19 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>388</v>
+        <v>767</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>spotify:track:3kNaNDh2G5Q9jAXpqoA51b</t>
+          <t>spotify:track:32VC4phBq8CWC3rFSnjEHr</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2020-03-30T21:19:03Z</t>
+          <t>2018-03-20T00:45:39Z</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1961,11 +1961,11 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>223448</v>
+        <v>400013</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1974,7 +1974,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>31.187.0.247</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1984,17 +1984,17 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>I Never Got Off The Bus</t>
+          <t>Take It Back</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Tebi Rex</t>
+          <t>Logic</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>The Young Will Eat The Old</t>
+          <t>Everybody</t>
         </is>
       </c>
       <c r="N18" t="inlineStr"/>
@@ -2018,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="V18" t="n">
-        <v>1585602917349</v>
+        <v>1521506340090</v>
       </c>
       <c r="W18" t="b">
         <v>0</v>
@@ -2026,19 +2026,19 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>404</v>
+        <v>804</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>spotify:track:45m6ioYnsSA5TeY6EE82Ha</t>
+          <t>spotify:track:7M1lOPZ7obkkzznia2OeVb</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2020-03-02T15:19:07Z</t>
+          <t>2018-03-20T11:24:27Z</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -2048,11 +2048,11 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>173357</v>
+        <v>312206</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>143.239.9.6</t>
+          <t>31.187.2.110</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -2071,17 +2071,17 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Dancing Bug</t>
+          <t>Black SpiderMan</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Le Boom</t>
+          <t>Logic</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>Dancing Bug</t>
+          <t>Everybody</t>
         </is>
       </c>
       <c r="N19" t="inlineStr"/>
@@ -2089,12 +2089,12 @@
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>clickrow</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>backbtn</t>
         </is>
       </c>
       <c r="S19" t="b">
@@ -2105,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="V19" t="n">
-        <v>1583162173916</v>
+        <v>1521506738196</v>
       </c>
       <c r="W19" t="b">
         <v>0</v>
@@ -2113,19 +2113,19 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>420</v>
+        <v>841</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>spotify:track:5ypOQL3PMZJoBkS2HMPCXO</t>
+          <t>spotify:track:67YkHJvLYOR1mKdpQSTsUr</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2020-04-17T00:46:57Z</t>
+          <t>2018-03-05T23:54:44Z</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -2135,11 +2135,11 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Windows 10 (10.0.16299; x64)</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>244148</v>
+        <v>260000</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -2148,7 +2148,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -2158,17 +2158,17 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Really Happy Aliens</t>
+          <t>Never Be Alone</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Fred V</t>
+          <t>TheFatRat</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Proximity</t>
+          <t>Never Be Alone</t>
         </is>
       </c>
       <c r="N20" t="inlineStr"/>
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="V20" t="n">
-        <v>1587084172222</v>
+        <v>1520293824240</v>
       </c>
       <c r="W20" t="b">
         <v>0</v>
@@ -2200,19 +2200,19 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>435</v>
+        <v>877</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>spotify:track:3tjwjBfPO1pyjhnrI0J5Nq</t>
+          <t>spotify:track:1XsN9Flu0VvZpXmrkBtZGt</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2020-04-13T20:05:34Z</t>
+          <t>2018-03-20T17:41:30Z</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -2222,11 +2222,11 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18363; x64; AppX)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>213132</v>
+        <v>211453</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>31.187.2.10</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2245,17 +2245,17 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Head First</t>
+          <t>Let’s Go</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Home</t>
+          <t>Stuck in the Sound</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Falling into Place</t>
+          <t>Pursuit</t>
         </is>
       </c>
       <c r="N21" t="inlineStr"/>
@@ -2263,7 +2263,7 @@
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>fwdbtn</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2279,7 +2279,7 @@
         <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>1586808120333</v>
+        <v>1521567478216</v>
       </c>
       <c r="W21" t="b">
         <v>0</v>
@@ -2287,19 +2287,19 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>449</v>
+        <v>912</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>spotify:track:3mxEfSqWVcQBHxMLHxv5r1</t>
+          <t>spotify:track:6gjbfsxdoNv7VZoAGRvIWf</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2020-03-15T14:01:29Z</t>
+          <t>2018-05-23T10:08:09Z</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -2309,11 +2309,11 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>590</v>
+        <v>231701</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -2322,7 +2322,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>31.187.0.229</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2332,17 +2332,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>I'm Not Human At All (Copenhagen X Sessions)</t>
+          <t>Metaphysical - Daktyl Remix</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Sleep Party People</t>
+          <t>Autograf</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>I'm Not Human At All (Copenhagen X Sessions)</t>
+          <t>Metaphysical (Daktyl Remix)</t>
         </is>
       </c>
       <c r="N22" t="inlineStr"/>
@@ -2355,18 +2355,18 @@
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>unexpected-exit-while-paused</t>
+          <t>endplay</t>
         </is>
       </c>
       <c r="S22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="b">
         <v>0</v>
       </c>
       <c r="V22" t="n">
-        <v>1584233209694</v>
+        <v>1527030213390</v>
       </c>
       <c r="W22" t="b">
         <v>0</v>
@@ -2374,19 +2374,19 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>463</v>
+        <v>947</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>spotify:track:7ympnDShDtkevRDPxMqPvR</t>
+          <t>spotify:track:4xKaAIRMff688GtmmDrvhh</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2020-05-10T21:03:55Z</t>
+          <t>2018-03-23T23:39:42Z</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -2396,11 +2396,11 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18362; x64; AppX)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>471946</v>
+        <v>672572</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2419,17 +2419,17 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Winter on the Weekend</t>
+          <t>Swim High</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Julia Stone</t>
+          <t>RIVKA</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>The Memory Machine</t>
+          <t>Faded</t>
         </is>
       </c>
       <c r="N23" t="inlineStr"/>
@@ -2437,7 +2437,7 @@
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>clickrow</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2453,7 +2453,7 @@
         <v>0</v>
       </c>
       <c r="V23" t="n">
-        <v>1589143516197</v>
+        <v>1521842463826</v>
       </c>
       <c r="W23" t="b">
         <v>0</v>
@@ -2461,19 +2461,19 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>477</v>
+        <v>981</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>spotify:track:3JvJupyJyXk9aWtSXyZqcc</t>
+          <t>spotify:track:7r5lF3RJeOo5CCDZStBrZf</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2020-03-22T21:05:22Z</t>
+          <t>2018-03-23T21:55:57Z</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2483,11 +2483,11 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>243000</v>
+        <v>395229</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -2496,7 +2496,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2506,17 +2506,17 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>holy terrain</t>
+          <t>4AM</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>FKA twigs</t>
+          <t>Vessels</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>MAGDALENE</t>
+          <t>Dilate</t>
         </is>
       </c>
       <c r="N24" t="inlineStr"/>
@@ -2540,7 +2540,7 @@
         <v>0</v>
       </c>
       <c r="V24" t="n">
-        <v>1584910878324</v>
+        <v>1521841762812</v>
       </c>
       <c r="W24" t="b">
         <v>0</v>
@@ -2548,19 +2548,19 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>490</v>
+        <v>1015</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>spotify:track:2tRMhAhbVKb3ay9lABihPt</t>
+          <t>spotify:track:2q3gxrNyZ1LPzGubB0Mg13</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2020-04-28T00:56:03Z</t>
+          <t>2018-03-14T13:48:23Z</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2570,11 +2570,11 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18362; x64; AppX)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>445735</v>
+        <v>175426</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -2583,7 +2583,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2593,17 +2593,17 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Epilogue</t>
+          <t>Warlord</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Weltmusik</t>
+          <t>What So Not</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Epilogue</t>
+          <t>Not All the Beautiful Things</t>
         </is>
       </c>
       <c r="N25" t="inlineStr"/>
@@ -2611,7 +2611,7 @@
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>clickrow</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2620,14 +2620,14 @@
         </is>
       </c>
       <c r="S25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="b">
         <v>0</v>
       </c>
       <c r="V25" t="n">
-        <v>1588034757064</v>
+        <v>1521035129428</v>
       </c>
       <c r="W25" t="b">
         <v>0</v>
@@ -2635,19 +2635,19 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>503</v>
+        <v>1048</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>spotify:track:4KfgBq7SrmjavjQS4ZQGHC</t>
+          <t>spotify:track:4qmvOVUt7U8szKXspAoLVy</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2020-03-22T21:09:49Z</t>
+          <t>2018-03-18T22:42:05Z</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -2657,40 +2657,40 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Partner google cast_tv;Chromecast;;2.0.0-342-92f0147--1.29.104827</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>255720</v>
+        <v>275175</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>ZZ</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Mozilla%2F5.0%20(X11;%20Linux%20armv7l)%20AppleWebKit%2F537.36%20(KHTML,%20like%20Gecko)%20Chrome%2F63.0.3239.58%20Safari%2F537.36%20CrKey%2F1.29.104827</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>sad day</t>
+          <t>I Am The Walrus - Remastered</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>FKA twigs</t>
+          <t>The Beatles</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>MAGDALENE</t>
+          <t>Magical Mystery Tour</t>
         </is>
       </c>
       <c r="N26" t="inlineStr"/>
@@ -2698,12 +2698,12 @@
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>unknown</t>
         </is>
       </c>
       <c r="S26" t="b">
@@ -2714,7 +2714,7 @@
         <v>0</v>
       </c>
       <c r="V26" t="n">
-        <v>1584911121767</v>
+        <v>0</v>
       </c>
       <c r="W26" t="b">
         <v>0</v>
@@ -2722,19 +2722,19 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>516</v>
+        <v>1080</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>spotify:track:1lCb4eleZgc8DKrv7MY21F</t>
+          <t>spotify:track:4EXRbn4TKJPh1B6kTtJSSf</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2020-03-02T15:29:26Z</t>
+          <t>2018-03-14T13:53:00Z</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -2744,11 +2744,11 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>244965</v>
+        <v>279360</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -2757,7 +2757,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>143.239.9.6</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2767,17 +2767,17 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>I Walk</t>
+          <t>We Keep on Running</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Æ MAK</t>
+          <t>What So Not</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>I Walk</t>
+          <t>Not All the Beautiful Things</t>
         </is>
       </c>
       <c r="N27" t="inlineStr"/>
@@ -2794,14 +2794,14 @@
         </is>
       </c>
       <c r="S27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="b">
         <v>0</v>
       </c>
       <c r="V27" t="n">
-        <v>1583162719310</v>
+        <v>1521035301918</v>
       </c>
       <c r="W27" t="b">
         <v>0</v>
@@ -2809,19 +2809,19 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>529</v>
+        <v>1112</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>spotify:track:24upABZ8A0sAepfu91sEYr</t>
+          <t>spotify:track:2cmRpmO04TLaKPzmAzySYZ</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2020-03-03T15:14:02Z</t>
+          <t>2018-03-02T10:00:08Z</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -2831,11 +2831,11 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>337314</v>
+        <v>103648</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -2844,7 +2844,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>143.239.9.6</t>
+          <t>31.187.2.61</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2854,17 +2854,17 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Moon (And It Went Like)</t>
+          <t>Dance Yrself Clean</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Kid Francescoli</t>
+          <t>LCD Soundsystem</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Play Me Again</t>
+          <t>This Is Happening</t>
         </is>
       </c>
       <c r="N28" t="inlineStr"/>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>logout</t>
+          <t>unexpected-exit-while-paused</t>
         </is>
       </c>
       <c r="S28" t="b">
@@ -2888,7 +2888,7 @@
         <v>0</v>
       </c>
       <c r="V28" t="n">
-        <v>1583227973011</v>
+        <v>1519957892657</v>
       </c>
       <c r="W28" t="b">
         <v>0</v>
@@ -2896,19 +2896,19 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>541</v>
+        <v>1144</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>spotify:track:7CVV0sfN38TC3c9DaxR2Tp</t>
+          <t>spotify:track:69Naniu2KjKjaQOBUagE8U</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2020-03-30T21:45:54Z</t>
+          <t>2018-04-16T21:49:19Z</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -2918,11 +2918,11 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Windows 10 (10.0.18362; x64; AppX)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>121470</v>
+        <v>215734</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -2931,7 +2931,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2941,17 +2941,17 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Antenna</t>
+          <t>Homemade Dynamite (Feat. Khalid, Post Malone &amp; SZA) - REMIX</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Citrus Fresh</t>
+          <t>Lorde</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Early Days/Late Nights</t>
+          <t>Homemade Dynamite (Feat. Khalid, Post Malone &amp; SZA) [REMIX]</t>
         </is>
       </c>
       <c r="N29" t="inlineStr"/>
@@ -2959,12 +2959,12 @@
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>fwdbtn</t>
+          <t>clickrow</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>endplay</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="S29" t="b">
@@ -2975,7 +2975,7 @@
         <v>0</v>
       </c>
       <c r="V29" t="n">
-        <v>1585601990213</v>
+        <v>1523915140605</v>
       </c>
       <c r="W29" t="b">
         <v>0</v>
@@ -2983,19 +2983,19 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>553</v>
+        <v>1176</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>spotify:track:6udA6tzAZ2bolSfaSibQEV</t>
+          <t>spotify:track:0b9oOr2ZgvyQu88wzixux9</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2020-03-09T21:42:30Z</t>
+          <t>2018-05-07T11:20:20Z</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -3005,11 +3005,11 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Android OS 8.0.0 API 26 (OnePlus, ONEPLUS A3003)</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>353407</v>
+        <v>225773</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -3018,7 +3018,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>109.255.113.201</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -3028,17 +3028,17 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Pay Phone</t>
+          <t>This Is America</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Fantom '87</t>
+          <t>Childish Gambino</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>Discovery</t>
+          <t>This Is America</t>
         </is>
       </c>
       <c r="N30" t="inlineStr"/>
@@ -3046,7 +3046,7 @@
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>fwdbtn</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3062,7 +3062,7 @@
         <v>0</v>
       </c>
       <c r="V30" t="n">
-        <v>1583789795250</v>
+        <v>1525691795218</v>
       </c>
       <c r="W30" t="b">
         <v>0</v>
@@ -3070,19 +3070,19 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>564</v>
+        <v>1207</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>spotify:track:7rWxjGLtUSmdr0d7X8L5Lq</t>
+          <t>spotify:track:3VAeTjREoKPY1exOXR4oBm</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2020-03-30T21:23:41Z</t>
+          <t>2018-04-30T23:10:05Z</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -3092,11 +3092,11 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Android OS 9 API 28 (OnePlus, ONEPLUS A3003)</t>
+          <t>Windows 10 (10.0.16299; x64)</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>91403</v>
+        <v>129599</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -3105,7 +3105,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>31.187.0.247</t>
+          <t>37.228.209.8</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -3115,17 +3115,17 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Men Are Trash</t>
+          <t>Go Fuck Yourself</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Tebi Rex</t>
+          <t>Two Feet</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Welcome to the Darkest Year of Our Adventures</t>
+          <t>First Steps</t>
         </is>
       </c>
       <c r="N31" t="inlineStr"/>
@@ -3133,12 +3133,12 @@
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>trackdone</t>
+          <t>fwdbtn</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>fwdbtn</t>
+          <t>trackdone</t>
         </is>
       </c>
       <c r="S31" t="b">
@@ -3149,7 +3149,7 @@
         <v>0</v>
       </c>
       <c r="V31" t="n">
-        <v>1585603325763</v>
+        <v>1525129299046</v>
       </c>
       <c r="W31" t="b">
         <v>0</v>

</xml_diff>